<commit_message>
fix 29.10.2024 price 15
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT-P,RDT-PH.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT-P,RDT-PH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8187022A-7DA1-4A00-93E6-507D1A44A77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCA14BC-B84B-4F19-862D-93CC5BC0D782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="7050" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
   <si>
     <t>В комплекте с регуляторами давления "после себя" поставляются:
 - с регуляторами давления "после себя" RDT-P: медная импульсная трубка - 1 шт.; латунная гайка - 2 шт.; латунный штуцер - 1 шт.
-- с регуляторами давления "после себя" RDT-T: медная импульсная трубка - 2 шт.; латунная гайка - 4 шт.; латунный штуцер - 1 шт.; охладитель импульса - 1 шт.</t>
+- с регуляторами давления "после себя" RDT-PH: медная импульсная трубка - 2 шт.; латунная гайка - 4 шт.; латунный штуцер - 1 шт.; охладитель импульса - 1 шт.</t>
   </si>
 </sst>
 </file>
@@ -428,9 +428,69 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -446,68 +506,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,7 +847,7 @@
   <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,12 +874,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -894,19 +894,19 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -921,19 +921,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -948,19 +948,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="43"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1000,12 +1000,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1027,19 +1027,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1054,19 +1054,19 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1081,18 +1081,18 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
       <c r="K10" s="5"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -1108,18 +1108,18 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="5"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -1135,19 +1135,19 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="2"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -1162,18 +1162,18 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
       <c r="K13" s="16"/>
       <c r="L13" s="2"/>
       <c r="M13" s="4"/>
@@ -1189,18 +1189,18 @@
       <c r="W13" s="4"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="16" t="s">
         <v>10</v>
       </c>
@@ -1218,19 +1218,19 @@
       <c r="W14" s="4"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="2"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1245,18 +1245,18 @@
       <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
       <c r="K16" s="16" t="s">
         <v>10</v>
       </c>
@@ -1274,18 +1274,18 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
       <c r="K17" s="16" t="s">
         <v>10</v>
       </c>
@@ -1303,18 +1303,18 @@
       <c r="W17" s="4"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
       <c r="K18" s="16"/>
       <c r="L18" s="2"/>
       <c r="M18" s="4"/>
@@ -1330,18 +1330,18 @@
       <c r="W18" s="4"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
       <c r="K19" s="16"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1382,12 +1382,12 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1409,19 +1409,19 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1436,19 +1436,19 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -1497,10 +1497,10 @@
       <c r="C25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="26"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="10" t="s">
         <v>29</v>
       </c>
@@ -1510,10 +1510,10 @@
       <c r="H25" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="26" t="s">
+      <c r="I25" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="43"/>
       <c r="K25" s="10" t="s">
         <v>2</v>
       </c>
@@ -1534,13 +1534,13 @@
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
       <c r="K26" s="10"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1637,10 +1637,10 @@
     <row r="30" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="14"/>
       <c r="G30" s="9" t="s">
         <v>11</v>
@@ -1665,10 +1665,10 @@
     <row r="31" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="38"/>
       <c r="F31" s="14"/>
       <c r="G31" s="9" t="s">
         <v>11</v>
@@ -1693,10 +1693,10 @@
     <row r="32" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="18"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="14"/>
       <c r="G32" s="9" t="s">
         <v>11</v>
@@ -1721,10 +1721,10 @@
     <row r="33" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="20"/>
+      <c r="E33" s="40"/>
       <c r="F33" s="15"/>
       <c r="G33" s="9" t="s">
         <v>15</v>
@@ -2607,13 +2607,28 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="A27:K27"/>
     <mergeCell ref="A28:K28"/>
     <mergeCell ref="E23:K23"/>
@@ -2630,28 +2645,13 @@
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A23:D23"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C5:K5"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>